<commit_message>
food environmental preprocess finished
</commit_message>
<xml_diff>
--- a/data/ad_hoc_data/food_items.xlsx
+++ b/data/ad_hoc_data/food_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pol.gil.figuerola\Documents\git\food-basket-cambodia-case-study\data\ad_hoc_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749F9855-193A-40FC-A88D-A8F16091576B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C073C76A-DAA6-464F-8A6E-0A3EF78C6036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="2415" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4320" yWindow="2565" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="108">
   <si>
     <t>Noodles, egg, dry, enriched</t>
   </si>
@@ -340,6 +340,21 @@
   </si>
   <si>
     <t>Banana flower heart</t>
+  </si>
+  <si>
+    <t>ENHANCE_ID</t>
+  </si>
+  <si>
+    <t>Food sub-group</t>
+  </si>
+  <si>
+    <t>Starchy staples</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>Animal source foods</t>
   </si>
 </sst>
 </file>
@@ -369,12 +384,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -389,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -401,6 +422,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -707,9 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -717,7 +740,7 @@
     <col min="2" max="2" width="10.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="40.28515625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" customWidth="1"/>
     <col min="7" max="8" width="20.28515625" customWidth="1"/>
   </cols>
@@ -735,8 +758,12 @@
       <c r="D1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
@@ -753,8 +780,12 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="E2" s="3">
+        <v>94850</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
@@ -771,8 +802,12 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="E3" s="3">
+        <v>94879</v>
+      </c>
+      <c r="F3" t="s">
+        <v>105</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
@@ -789,8 +824,12 @@
       <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="3">
+        <v>104945</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
@@ -807,8 +846,12 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="3">
+        <v>66362</v>
+      </c>
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
@@ -825,8 +868,12 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="3">
+        <v>56375</v>
+      </c>
+      <c r="F6" t="s">
+        <v>105</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
@@ -843,8 +890,12 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="3">
+        <v>16440</v>
+      </c>
+      <c r="F7" t="s">
+        <v>105</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
@@ -861,8 +912,12 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="3">
+        <v>16446</v>
+      </c>
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -879,8 +934,12 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="3">
+        <v>106464</v>
+      </c>
+      <c r="F9" t="s">
+        <v>105</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
@@ -897,8 +956,12 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="3">
+        <v>96496</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
@@ -915,8 +978,12 @@
       <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="3">
+        <v>65322</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
@@ -933,8 +1000,12 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="3">
+        <v>55340</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
@@ -951,8 +1022,12 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="E13" s="3">
+        <v>55388</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
@@ -969,8 +1044,12 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="E14" s="3">
+        <v>55519</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -987,8 +1066,12 @@
       <c r="D15" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="3">
+        <v>15557</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
@@ -1005,8 +1088,12 @@
       <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="E16" s="3">
+        <v>55573</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
@@ -1023,8 +1110,12 @@
       <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="E17" s="3">
+        <v>56661</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
@@ -1041,8 +1132,12 @@
       <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="E18" s="3">
+        <v>96689</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
@@ -1059,8 +1154,12 @@
       <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="E19" s="3">
+        <v>96713</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
@@ -1077,8 +1176,12 @@
       <c r="D20" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="3">
+        <v>96715</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
@@ -1095,8 +1198,12 @@
       <c r="D21" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="E21" s="3">
+        <v>56716</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
@@ -1113,8 +1220,12 @@
       <c r="D22" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="E22" s="3">
+        <v>56746</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
@@ -1131,8 +1242,12 @@
       <c r="D23" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="E23" s="3">
+        <v>56757</v>
+      </c>
+      <c r="F23" t="s">
+        <v>18</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
@@ -1149,8 +1264,12 @@
       <c r="D24" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="E24" s="3">
+        <v>56787</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
@@ -1167,8 +1286,12 @@
       <c r="D25" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="E25" s="3">
+        <v>56796</v>
+      </c>
+      <c r="F25" t="s">
+        <v>18</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
@@ -1185,8 +1308,12 @@
       <c r="D26" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="E26" s="3">
+        <v>96797</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
@@ -1203,8 +1330,12 @@
       <c r="D27" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="E27" s="3">
+        <v>16822</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
@@ -1221,8 +1352,12 @@
       <c r="D28" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="E28" s="3">
+        <v>16832</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
@@ -1239,8 +1374,12 @@
       <c r="D29" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="E29" s="3">
+        <v>16835</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
@@ -1257,8 +1396,12 @@
       <c r="D30" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="E30" s="3">
+        <v>56839</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
@@ -1275,8 +1418,12 @@
       <c r="D31" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="E31" s="3">
+        <v>1332</v>
+      </c>
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
@@ -1293,8 +1440,12 @@
       <c r="D32" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="E32" s="3">
+        <v>96849</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
@@ -1311,8 +1462,12 @@
       <c r="D33" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="E33" s="3">
+        <v>16872</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
@@ -1329,8 +1484,12 @@
       <c r="D34" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="E34" s="3">
+        <v>96876</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
@@ -1347,8 +1506,12 @@
       <c r="D35" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="E35" s="3">
+        <v>16938</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
@@ -1365,8 +1528,12 @@
       <c r="D36" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="E36" s="3">
+        <v>56957</v>
+      </c>
+      <c r="F36" t="s">
+        <v>18</v>
+      </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
@@ -1383,8 +1550,12 @@
       <c r="D37" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="E37" s="3">
+        <v>96986</v>
+      </c>
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
@@ -1401,8 +1572,12 @@
       <c r="D38" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="E38" s="3">
+        <v>17000</v>
+      </c>
+      <c r="F38" t="s">
+        <v>18</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
@@ -1419,8 +1594,12 @@
       <c r="D39" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="E39" s="3">
+        <v>97083</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
+      </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
@@ -1437,8 +1616,12 @@
       <c r="D40" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+      <c r="E40" s="3">
+        <v>97084</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
@@ -1455,8 +1638,12 @@
       <c r="D41" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="E41" s="3">
+        <v>17114</v>
+      </c>
+      <c r="F41" t="s">
+        <v>18</v>
+      </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
@@ -1473,8 +1660,12 @@
       <c r="D42" t="s">
         <v>18</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="E42" s="3">
+        <v>57123</v>
+      </c>
+      <c r="F42" t="s">
+        <v>18</v>
+      </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
@@ -1491,8 +1682,12 @@
       <c r="D43" t="s">
         <v>18</v>
       </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="E43" s="3">
+        <v>57147</v>
+      </c>
+      <c r="F43" t="s">
+        <v>18</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
@@ -1509,8 +1704,12 @@
       <c r="D44" t="s">
         <v>18</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="E44" s="3">
+        <v>17166</v>
+      </c>
+      <c r="F44" t="s">
+        <v>18</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
@@ -1527,8 +1726,12 @@
       <c r="D45" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
+      <c r="E45" s="3">
+        <v>57173</v>
+      </c>
+      <c r="F45" t="s">
+        <v>18</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
@@ -1545,8 +1748,12 @@
       <c r="D46" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="E46" s="3">
+        <v>17258</v>
+      </c>
+      <c r="F46" t="s">
+        <v>18</v>
+      </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
@@ -1563,8 +1770,12 @@
       <c r="D47" t="s">
         <v>49</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+      <c r="E47" s="3">
+        <v>44288</v>
+      </c>
+      <c r="F47" t="s">
+        <v>106</v>
+      </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
@@ -1581,8 +1792,12 @@
       <c r="D48" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
+      <c r="E48" s="3">
+        <v>54401</v>
+      </c>
+      <c r="F48" t="s">
+        <v>106</v>
+      </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
@@ -1599,8 +1814,12 @@
       <c r="D49" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
+      <c r="E49" s="3">
+        <v>14415</v>
+      </c>
+      <c r="F49" t="s">
+        <v>106</v>
+      </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
@@ -1617,8 +1836,12 @@
       <c r="D50" t="s">
         <v>49</v>
       </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
+      <c r="E50" s="3">
+        <v>44493</v>
+      </c>
+      <c r="F50" t="s">
+        <v>106</v>
+      </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
@@ -1635,8 +1858,12 @@
       <c r="D51" t="s">
         <v>49</v>
       </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
+      <c r="E51" s="3">
+        <v>54499</v>
+      </c>
+      <c r="F51" t="s">
+        <v>106</v>
+      </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
@@ -1653,8 +1880,12 @@
       <c r="D52" t="s">
         <v>49</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="E52" s="3">
+        <v>14526</v>
+      </c>
+      <c r="F52" t="s">
+        <v>106</v>
+      </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
@@ -1671,8 +1902,12 @@
       <c r="D53" t="s">
         <v>49</v>
       </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
+      <c r="E53" s="3">
+        <v>14540</v>
+      </c>
+      <c r="F53" t="s">
+        <v>106</v>
+      </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
@@ -1689,8 +1924,12 @@
       <c r="D54" t="s">
         <v>49</v>
       </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
+      <c r="E54" s="3">
+        <v>14574</v>
+      </c>
+      <c r="F54" t="s">
+        <v>106</v>
+      </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
@@ -1707,8 +1946,12 @@
       <c r="D55" t="s">
         <v>49</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
+      <c r="E55" s="3">
+        <v>74618</v>
+      </c>
+      <c r="F55" t="s">
+        <v>106</v>
+      </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
@@ -1725,8 +1968,12 @@
       <c r="D56" t="s">
         <v>49</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
+      <c r="E56" s="3">
+        <v>17246</v>
+      </c>
+      <c r="F56" t="s">
+        <v>106</v>
+      </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
@@ -1743,8 +1990,12 @@
       <c r="D57" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
+      <c r="E57" s="3">
+        <v>55595</v>
+      </c>
+      <c r="F57" t="s">
+        <v>107</v>
+      </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
@@ -1761,8 +2012,12 @@
       <c r="D58" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
+      <c r="E58" s="3">
+        <v>15638</v>
+      </c>
+      <c r="F58" t="s">
+        <v>107</v>
+      </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
@@ -1779,8 +2034,12 @@
       <c r="D59" t="s">
         <v>60</v>
       </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
+      <c r="E59" s="3">
+        <v>15650</v>
+      </c>
+      <c r="F59" t="s">
+        <v>107</v>
+      </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
@@ -1797,8 +2056,12 @@
       <c r="D60" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
+      <c r="E60" s="3">
+        <v>15771</v>
+      </c>
+      <c r="F60" t="s">
+        <v>107</v>
+      </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
@@ -1815,8 +2078,12 @@
       <c r="D61" t="s">
         <v>60</v>
       </c>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
+      <c r="E61" s="3">
+        <v>55774</v>
+      </c>
+      <c r="F61" t="s">
+        <v>107</v>
+      </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
@@ -1833,8 +2100,12 @@
       <c r="D62" t="s">
         <v>60</v>
       </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
+      <c r="E62" s="3">
+        <v>95808</v>
+      </c>
+      <c r="F62" t="s">
+        <v>107</v>
+      </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
@@ -1851,8 +2122,12 @@
       <c r="D63" t="s">
         <v>60</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
+      <c r="E63" s="3">
+        <v>15823</v>
+      </c>
+      <c r="F63" t="s">
+        <v>107</v>
+      </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
@@ -1869,8 +2144,12 @@
       <c r="D64" t="s">
         <v>60</v>
       </c>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
+      <c r="E64" s="3">
+        <v>95957</v>
+      </c>
+      <c r="F64" t="s">
+        <v>107</v>
+      </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
@@ -1887,8 +2166,12 @@
       <c r="D65" t="s">
         <v>60</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
+      <c r="E65" s="3">
+        <v>95977</v>
+      </c>
+      <c r="F65" t="s">
+        <v>107</v>
+      </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
@@ -1905,8 +2188,12 @@
       <c r="D66" t="s">
         <v>60</v>
       </c>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
+      <c r="E66" s="3">
+        <v>96004</v>
+      </c>
+      <c r="F66" t="s">
+        <v>107</v>
+      </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
@@ -1923,8 +2210,12 @@
       <c r="D67" t="s">
         <v>60</v>
       </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
+      <c r="E67" s="3">
+        <v>55840</v>
+      </c>
+      <c r="F67" t="s">
+        <v>107</v>
+      </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
@@ -1941,8 +2232,12 @@
       <c r="D68" t="s">
         <v>60</v>
       </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
+      <c r="E68" s="3">
+        <v>56026</v>
+      </c>
+      <c r="F68" t="s">
+        <v>107</v>
+      </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
@@ -1959,8 +2254,12 @@
       <c r="D69" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
+      <c r="E69" s="3">
+        <v>13826</v>
+      </c>
+      <c r="F69" t="s">
+        <v>107</v>
+      </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
@@ -1977,8 +2276,12 @@
       <c r="D70" t="s">
         <v>73</v>
       </c>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
+      <c r="E70" s="3">
+        <v>103879</v>
+      </c>
+      <c r="F70" t="s">
+        <v>107</v>
+      </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
@@ -1995,8 +2298,12 @@
       <c r="D71" t="s">
         <v>73</v>
       </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
+      <c r="E71" s="3">
+        <v>13909</v>
+      </c>
+      <c r="F71" t="s">
+        <v>107</v>
+      </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
@@ -2013,8 +2320,12 @@
       <c r="D72" t="s">
         <v>73</v>
       </c>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
+      <c r="E72" s="3">
+        <v>13928</v>
+      </c>
+      <c r="F72" t="s">
+        <v>107</v>
+      </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
@@ -2031,8 +2342,12 @@
       <c r="D73" t="s">
         <v>73</v>
       </c>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
+      <c r="E73" s="3">
+        <v>74111</v>
+      </c>
+      <c r="F73" t="s">
+        <v>107</v>
+      </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
@@ -2049,8 +2364,12 @@
       <c r="D74" t="s">
         <v>73</v>
       </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
+      <c r="E74" s="3">
+        <v>54117</v>
+      </c>
+      <c r="F74" t="s">
+        <v>107</v>
+      </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
@@ -2067,8 +2386,12 @@
       <c r="D75" t="s">
         <v>73</v>
       </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
+      <c r="E75" s="3">
+        <v>14121</v>
+      </c>
+      <c r="F75" t="s">
+        <v>107</v>
+      </c>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
@@ -2085,8 +2408,12 @@
       <c r="D76" t="s">
         <v>73</v>
       </c>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
+      <c r="E76" s="3">
+        <v>54151</v>
+      </c>
+      <c r="F76" t="s">
+        <v>107</v>
+      </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
@@ -2103,8 +2430,12 @@
       <c r="D77" t="s">
         <v>73</v>
       </c>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
+      <c r="E77" s="3">
+        <v>94153</v>
+      </c>
+      <c r="F77" t="s">
+        <v>107</v>
+      </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
@@ -2121,8 +2452,12 @@
       <c r="D78" t="s">
         <v>73</v>
       </c>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
+      <c r="E78" s="3">
+        <v>54233</v>
+      </c>
+      <c r="F78" t="s">
+        <v>107</v>
+      </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
@@ -2139,8 +2474,12 @@
       <c r="D79" t="s">
         <v>73</v>
       </c>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
+      <c r="E79" s="3">
+        <v>54240</v>
+      </c>
+      <c r="F79" t="s">
+        <v>107</v>
+      </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
@@ -2157,8 +2496,12 @@
       <c r="D80" t="s">
         <v>85</v>
       </c>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
+      <c r="E80" s="3">
+        <v>76198</v>
+      </c>
+      <c r="F80" t="s">
+        <v>107</v>
+      </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
@@ -2175,8 +2518,12 @@
       <c r="D81" t="s">
         <v>85</v>
       </c>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
+      <c r="E81" s="3">
+        <v>26236</v>
+      </c>
+      <c r="F81" t="s">
+        <v>107</v>
+      </c>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
@@ -2193,8 +2540,12 @@
       <c r="D82" t="s">
         <v>88</v>
       </c>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
+      <c r="E82" s="3">
+        <v>13726</v>
+      </c>
+      <c r="F82" t="s">
+        <v>107</v>
+      </c>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
@@ -2211,8 +2562,12 @@
       <c r="D83" t="s">
         <v>88</v>
       </c>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
+      <c r="E83" s="3">
+        <v>13740</v>
+      </c>
+      <c r="F83" t="s">
+        <v>107</v>
+      </c>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
@@ -2229,8 +2584,12 @@
       <c r="D84" t="s">
         <v>91</v>
       </c>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
+      <c r="E84" s="3">
+        <v>56244</v>
+      </c>
+      <c r="F84" t="s">
+        <v>91</v>
+      </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
@@ -2247,8 +2606,12 @@
       <c r="D85" t="s">
         <v>91</v>
       </c>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
+      <c r="E85" s="3">
+        <v>96320</v>
+      </c>
+      <c r="F85" t="s">
+        <v>91</v>
+      </c>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
@@ -2265,8 +2628,10 @@
       <c r="D86" t="s">
         <v>94</v>
       </c>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
+      <c r="E86" s="3">
+        <v>56571</v>
+      </c>
+      <c r="F86" s="6"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
@@ -2283,8 +2648,10 @@
       <c r="D87" t="s">
         <v>94</v>
       </c>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
+      <c r="E87" s="3">
+        <v>16574</v>
+      </c>
+      <c r="F87" s="6"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
@@ -2301,8 +2668,10 @@
       <c r="D88" t="s">
         <v>97</v>
       </c>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
+      <c r="E88" s="3">
+        <v>55236</v>
+      </c>
+      <c r="F88" s="6"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>

</xml_diff>